<commit_message>
Adição de mais 3 meses aos dados
</commit_message>
<xml_diff>
--- a/MassaRendimento.xlsx
+++ b/MassaRendimento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Tabela 6423 - Massa de rendimento, real e nominal do trabalho principal, efetivamente recebido no mês de referência, pelas pessoas de 14 anos ou mais de idade, empregadas no trabalho principal da semana de referência, com rendimento do trabalho principal - Total, coeficiente de variação, variações percentuais e absolutas em relação aos três trimestres móveis anteriores e ao mesmo trimestre móvel do ano anterior, e média anual</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>mai-jun-jul 2020</t>
+  </si>
+  <si>
+    <t>jun-jul-ago 2020</t>
+  </si>
+  <si>
+    <t>jul-ago-set 2020</t>
+  </si>
+  <si>
+    <t>ago-set-out 2020</t>
   </si>
   <si>
     <t>Brasil</t>
@@ -233,7 +242,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -335,10 +344,19 @@
       <c r="Z4" t="s">
         <v>27</v>
       </c>
+      <c r="AA4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>148006</v>
@@ -415,19 +433,28 @@
       <c r="Z5">
         <v>137654</v>
       </c>
+      <c r="AA5">
+        <v>137510</v>
+      </c>
+      <c r="AB5">
+        <v>139961</v>
+      </c>
+      <c r="AC5">
+        <v>141908</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:Z1"/>
-    <mergeCell ref="A2:Z2"/>
+    <mergeCell ref="A1:AC1"/>
+    <mergeCell ref="A2:AC2"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:Z3"/>
-    <mergeCell ref="A6:Z6"/>
+    <mergeCell ref="B3:AC3"/>
+    <mergeCell ref="A6:AC6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -445,12 +472,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -460,63 +487,63 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>